<commit_message>
add ExcelUser, CSVUser, etc.
</commit_message>
<xml_diff>
--- a/src/test/resources/allUsers.xlsx
+++ b/src/test/resources/allUsers.xlsx
@@ -16,23 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>qwerty</t>
   </si>
   <si>
-    <t>mail@gmail.com</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>ivanka</t>
   </si>
   <si>
@@ -45,13 +33,37 @@
     <t>Administrator</t>
   </si>
   <si>
-    <t>firstName1</t>
-  </si>
-  <si>
-    <t>lastName1</t>
-  </si>
-  <si>
-    <t>login1</t>
+    <t>aaaa@gmail.com</t>
+  </si>
+  <si>
+    <t>myroslava</t>
+  </si>
+  <si>
+    <t>myroslav</t>
+  </si>
+  <si>
+    <t>shram</t>
+  </si>
+  <si>
+    <t>gmail@gmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>Login Name</t>
   </si>
 </sst>
 </file>
@@ -394,66 +406,69 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>

</xml_diff>